<commit_message>
Created a new graph and added use of medication to the 'important variables' list. Added csvs of tests to place into the report
</commit_message>
<xml_diff>
--- a/Datasets/Indices of fit for all models.xlsx
+++ b/Datasets/Indices of fit for all models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdullahiqbal/Desktop/Documents/Dat5902FinalProject/dat5902Project/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB5465E4-AFC4-4D4D-BDF1-222EC85C1308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8682F94-1495-D74B-B854-E0447654DF6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20780" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{22075999-EF60-EE4E-8665-74046C2C998A}"/>
+    <workbookView xWindow="11580" yWindow="5060" windowWidth="27640" windowHeight="16940" xr2:uid="{22075999-EF60-EE4E-8665-74046C2C998A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="15">
   <si>
     <t>Value</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>LogLik</t>
-  </si>
-  <si>
-    <t>chi2p-value</t>
   </si>
   <si>
     <t>chi2 Baseline</t>
@@ -119,8 +116,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,7 +456,7 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="I2" sqref="I2:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -477,10 +475,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -521,40 +519,40 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <v>33.713104000000001</v>
-      </c>
-      <c r="E2">
-        <v>3.0000000000000001E-6</v>
+        <v>48.655132999999999</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2.6102179999999999E-9</v>
       </c>
       <c r="F2">
-        <v>149.49676400000001</v>
+        <v>98.099002999999996</v>
       </c>
       <c r="G2">
-        <v>0.79707600000000001</v>
+        <v>0.51547600000000005</v>
       </c>
       <c r="H2">
-        <v>0.77448899999999998</v>
+        <v>0.50402000000000002</v>
       </c>
       <c r="I2">
-        <v>0.63918299999999995</v>
+        <v>0.206432</v>
       </c>
       <c r="J2">
-        <v>0.77448899999999998</v>
+        <v>0.50402000000000002</v>
       </c>
       <c r="K2">
-        <v>0.67532099999999995</v>
+        <v>0.22476199999999999</v>
       </c>
       <c r="L2">
-        <v>0.266264</v>
+        <v>0.32831500000000002</v>
       </c>
       <c r="M2">
-        <v>9.1777289999999994</v>
+        <v>8.8132889999999993</v>
       </c>
       <c r="N2">
-        <v>21.211324999999999</v>
+        <v>20.846886000000001</v>
       </c>
       <c r="O2">
-        <v>0.41113499999999997</v>
+        <v>0.59335499999999997</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -568,10 +566,10 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
@@ -659,10 +657,10 @@
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s">
         <v>4</v>
@@ -703,40 +701,40 @@
         <v>7</v>
       </c>
       <c r="D10">
-        <v>9.0116239999999994</v>
+        <v>7.262365</v>
       </c>
       <c r="E10">
-        <v>2.9137E-2</v>
+        <v>6.3989000000000004E-2</v>
       </c>
       <c r="F10">
-        <v>152.00415100000001</v>
+        <v>100.60639</v>
       </c>
       <c r="G10">
-        <v>0.95854200000000001</v>
+        <v>0.95446500000000001</v>
       </c>
       <c r="H10">
-        <v>0.94071499999999997</v>
+        <v>0.92781400000000003</v>
       </c>
       <c r="I10">
-        <v>0.86166699999999996</v>
+        <v>0.83156600000000003</v>
       </c>
       <c r="J10">
-        <v>0.94071499999999997</v>
+        <v>0.92781400000000003</v>
       </c>
       <c r="K10">
-        <v>0.90326399999999996</v>
+        <v>0.89375199999999999</v>
       </c>
       <c r="L10">
-        <v>0.15728700000000001</v>
+        <v>0.132441</v>
       </c>
       <c r="M10">
-        <v>13.780203999999999</v>
+        <v>13.822869000000001</v>
       </c>
       <c r="N10">
-        <v>30.627238999999999</v>
+        <v>30.669903999999999</v>
       </c>
       <c r="O10">
-        <v>0.109898</v>
+        <v>8.8565000000000005E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>